<commit_message>
Adding results of a properly powered investigation of Psychological Science (the Journal)'s recent policies re: sample size determination
</commit_message>
<xml_diff>
--- a/PowerAnalysesPsycSci.xlsx
+++ b/PowerAnalysesPsycSci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Effect Size paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1521DD-D223-4C05-B6B3-B66197DA81A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3A9493-D628-4017-AD19-025DEA80CF18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6030" xr2:uid="{7DCA936C-81AC-45A1-865F-1271D14B61EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6030" xr2:uid="{7DCA936C-81AC-45A1-865F-1271D14B61EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,9 +467,6 @@
     <t>Infectious Disease and Imperfections of Self-Image Joshua M. Ackerman, Joshua M. Tybur, Chad R. Mortensen,</t>
   </si>
   <si>
-    <t>To determine sufficiently powered sample sizes in the following studies, we reviewed effect sizes of several previous tests of experimentally manipulated pathogen cues on responses to appearance-relevant stimuli (Ackerman et al., 2009; Miller &amp; Maner, 2012; White et al., 2013). We observed an average d of 0.65.</t>
-  </si>
-  <si>
     <t>Mothers’ Neural and Behavioral Responses to Their Infants’ Distress Cues: The Role of Secure Base Script Knowledge Ashley M. Groh, Katherine C. Haydon,</t>
   </si>
   <si>
@@ -563,9 +560,6 @@
     <t xml:space="preserve"> We preselected a sample size approximately double those used in our prior studies (e.g., Smallwood et al., 2016). A sample size of at least 125 is recommended in order to have 95% confidence that a correlation of typical size (r = .20–.30) is present and greater than 0 (Hemphill, 2003).</t>
   </si>
   <si>
-    <t xml:space="preserve">No previous studies have reported effects of in-group (vs. out-group) affiliation on P3 responses. Thus, sample size was estimated from power calculations based on effect sizes from prior studies using similar alcohol cue-presentation paradigms and predicting alcohol use prospectively with alcohol-cue-elicited P3 amplitude (e.g., Bartholow et al., 2007; Bartholow, Lust, &amp; Tragesser, 2010). </t>
-  </si>
-  <si>
     <t>Average effect size in a set of studies (not a formal meta-analysis)</t>
   </si>
   <si>
@@ -726,6 +720,12 @@
   </si>
   <si>
     <t>Sample size for both studies was determined a priori to be 50 participants per condition, a sample size comparable with that of a similarly designed experiment (Dougherty et al., 2005).</t>
+  </si>
+  <si>
+    <t>es. Thus, sample size was estimated from power calculations based on effect sizes from prior studies using similar alcohol cuepresentation paradigms and predicting alcohol use prospectively with alcohol-cue-elicited P3 amplitude (e.g., Bartholow et al., 2007; Bartholow, Lust, &amp; Tragesser, 2010). However, because effect sizes in those prior studies (e.g., d = 0.89, partial R2 = .09) were likely overestimated because of small sample sizes (Ns = 46), we sought here to more than double the sample size to help ensure more accurate estimates.</t>
+  </si>
+  <si>
+    <t>To determine sufficiently powered sample sizes in the following studies, we reviewed effect sizes of several previous tests of experimentally manipulated pathogen cues on responses to appearance-relevant stimuli (Ackerman et al., 2009; Miller &amp; Maner, 2012; White et al., 2013). We observed an average d of 0.65. To compensate for potential effect-size inflation, we estimated a d of 0.45, which is closer to effect sizes obtained by field-wide meta-analyses (Richard, Bond, &amp; Stokes-Zoota, 2003). This suggested that a sample size of 158 would be needed to detect an effect with 80% power.</t>
   </si>
 </sst>
 </file>
@@ -1080,13 +1080,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E518BE-25CC-4B16-883C-FB193D628AE7}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="96" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="96" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1106,10 +1106,10 @@
         <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>125</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>127</v>
       </c>
       <c r="D64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2321,7 +2321,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>137</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2449,7 +2449,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2520,7 +2520,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -2528,10 +2528,10 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -2543,15 +2543,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
         <v>146</v>
-      </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77" t="s">
-        <v>147</v>
       </c>
       <c r="F77" t="s">
         <v>77</v>
@@ -2560,9 +2560,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -2574,18 +2574,18 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
         <v>150</v>
       </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>151</v>
-      </c>
-      <c r="D79" t="s">
-        <v>152</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2597,9 +2597,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -2611,15 +2611,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
         <v>154</v>
-      </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-      <c r="C81" t="s">
-        <v>155</v>
       </c>
       <c r="D81" t="s">
         <v>87</v>
@@ -2634,15 +2634,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
         <v>156</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82" t="s">
-        <v>157</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2654,18 +2654,18 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
+        <v>170</v>
+      </c>
+      <c r="D83" t="s">
         <v>171</v>
-      </c>
-      <c r="D83" t="s">
-        <v>172</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2677,15 +2677,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F84" t="s">
         <v>76</v>
@@ -2694,15 +2694,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F85" t="s">
         <v>76</v>
@@ -2711,15 +2711,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2731,15 +2731,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F87" t="s">
         <v>76</v>
@@ -2748,9 +2748,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -2762,18 +2762,18 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" t="s">
+        <v>230</v>
+      </c>
+      <c r="D89" t="s">
         <v>177</v>
-      </c>
-      <c r="D89" t="s">
-        <v>179</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -2785,15 +2785,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F90" t="s">
         <v>76</v>
@@ -2802,15 +2802,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F91" t="s">
         <v>76</v>
@@ -2819,15 +2819,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F92" t="s">
         <v>76</v>
@@ -2836,15 +2836,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D93" t="s">
         <v>97</v>
@@ -2859,18 +2859,18 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D94" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -2882,15 +2882,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F95" t="s">
         <v>76</v>
@@ -2899,43 +2899,43 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G96">
         <v>2017</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G97">
         <v>2017</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D98" t="s">
         <v>29</v>
@@ -2944,38 +2944,38 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G98">
         <v>2017</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F99" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G99">
         <v>2017</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D100" t="s">
         <v>60</v>
@@ -2984,21 +2984,21 @@
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G100">
         <v>2017</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D101" t="s">
         <v>53</v>
@@ -3007,97 +3007,97 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G101">
         <v>2017</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G102">
         <v>2017</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F103" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G103">
         <v>2017</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F104" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G104">
         <v>2017</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G105">
         <v>2017</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G106">
         <v>2017</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D107" t="s">
         <v>29</v>
@@ -3106,35 +3106,35 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G107">
         <v>2017</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G108">
         <v>2017</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D109" t="s">
         <v>87</v>
@@ -3143,49 +3143,49 @@
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G109">
         <v>2017</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="F110" t="s">
         <v>200</v>
-      </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-      <c r="F110" t="s">
-        <v>202</v>
       </c>
       <c r="G110">
         <v>2017</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="F111" t="s">
         <v>211</v>
-      </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
-      <c r="F111" t="s">
-        <v>213</v>
       </c>
       <c r="G111">
         <v>2017</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D112" t="s">
         <v>29</v>
@@ -3194,69 +3194,69 @@
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G112">
         <v>2017</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G113">
         <v>2017</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G114">
         <v>2017</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G115">
         <v>2017</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D116" t="s">
         <v>97</v>
@@ -3265,35 +3265,35 @@
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G116">
         <v>2017</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="F117" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G117">
         <v>2017</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D118" t="s">
         <v>29</v>
@@ -3302,75 +3302,75 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G118">
         <v>2017</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F119" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G119">
         <v>2017</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B120">
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D120" t="s">
         <v>87</v>
       </c>
       <c r="F120" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G120">
         <v>2017</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="F121" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G121">
         <v>2017</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F122" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G122">
         <v>2017</v>

</xml_diff>